<commit_message>
extra overige task toegevoegd
</commit_message>
<xml_diff>
--- a/Documenten EenmaalAndermaal/Sprint voortgang/burndownchart.xlsx
+++ b/Documenten EenmaalAndermaal/Sprint voortgang/burndownchart.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheng\Documents\GitHub\I-Project\Documenten EenmaalAndermaal\Sprint voortgang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peiwand\Documents\GitHub\I-Project\Documenten EenmaalAndermaal\Sprint voortgang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8166BB52-3756-4B09-9EC5-3747B93DAF8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8607DA7B-8827-43D2-9EDB-90E2182EC77A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{DDF3D36C-582C-41B2-A361-11FA0D75ED19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DDF3D36C-582C-41B2-A361-11FA0D75ED19}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Taken</t>
   </si>
@@ -225,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve"> + tijd voor alle ontwerpen/testcases/pseudo code</t>
+  </si>
+  <si>
+    <t>In beheersomgeving gebruikers die verkoper willen worden goed kunnen keuren</t>
   </si>
 </sst>
 </file>
@@ -306,7 +311,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -322,7 +327,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -618,23 +623,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341DCF5F-E2BF-41A3-B0D1-762933A4747F}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -654,14 +659,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -674,7 +679,7 @@
       </c>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -685,7 +690,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -696,7 +701,7 @@
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -707,7 +712,7 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -718,7 +723,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -729,7 +734,7 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -740,7 +745,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -751,7 +756,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -762,7 +767,7 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -773,7 +778,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -782,7 +787,7 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -793,7 +798,7 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -804,7 +809,7 @@
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -814,7 +819,7 @@
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -824,14 +829,14 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -841,14 +846,14 @@
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -858,7 +863,7 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>23</v>
       </c>
@@ -868,7 +873,7 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>24</v>
       </c>
@@ -878,7 +883,7 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -888,11 +893,11 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -902,7 +907,7 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
@@ -912,14 +917,14 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>26</v>
       </c>
@@ -929,7 +934,7 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>27</v>
       </c>
@@ -939,7 +944,7 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
@@ -949,7 +954,7 @@
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>28</v>
       </c>
@@ -959,14 +964,14 @@
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
     </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>57</v>
       </c>
@@ -976,7 +981,7 @@
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
     </row>
-    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>30</v>
       </c>
@@ -989,7 +994,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>31</v>
       </c>
@@ -999,7 +1004,7 @@
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>32</v>
       </c>
@@ -1009,7 +1014,7 @@
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
     </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>33</v>
       </c>
@@ -1019,14 +1024,14 @@
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
     </row>
-    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>35</v>
       </c>
@@ -1036,7 +1041,7 @@
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>36</v>
       </c>
@@ -1046,7 +1051,7 @@
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
     </row>
-    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>37</v>
       </c>
@@ -1056,14 +1061,14 @@
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>39</v>
       </c>
@@ -1073,7 +1078,7 @@
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>60</v>
       </c>
@@ -1083,7 +1088,7 @@
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
     </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>40</v>
       </c>
@@ -1093,14 +1098,14 @@
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
     </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -1110,7 +1115,7 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>44</v>
       </c>
@@ -1120,7 +1125,7 @@
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
     </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>62</v>
       </c>
@@ -1130,7 +1135,7 @@
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>45</v>
       </c>
@@ -1140,7 +1145,7 @@
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
     </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>46</v>
       </c>
@@ -1150,7 +1155,7 @@
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
     </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>47</v>
       </c>
@@ -1160,7 +1165,7 @@
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>48</v>
       </c>
@@ -1170,7 +1175,7 @@
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
     </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>49</v>
       </c>
@@ -1180,7 +1185,7 @@
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
@@ -1190,12 +1195,20 @@
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
     </row>
-    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="13">
-        <f>SUM(B2:B56)</f>
-        <v>86</v>
-      </c>
-      <c r="D58" s="11" t="s">
+    <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B65" s="13">
+        <f>SUM(B2:B57)</f>
+        <v>90</v>
+      </c>
+      <c r="D65" s="11" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
taak toegevoegd bij story 5
</commit_message>
<xml_diff>
--- a/Documenten EenmaalAndermaal/Sprint voortgang/burndownchart.xlsx
+++ b/Documenten EenmaalAndermaal/Sprint voortgang/burndownchart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peiwand\Documents\GitHub\I-Project\Documenten EenmaalAndermaal\Sprint voortgang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\Iproject\github\I-Project\Documenten EenmaalAndermaal\Sprint voortgang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969FA8D4-71E4-42F4-A51F-B65F8C643A68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D5C9E1-1F9A-4F39-9388-4D5D16234AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DDF3D36C-582C-41B2-A361-11FA0D75ED19}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{DDF3D36C-582C-41B2-A361-11FA0D75ED19}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Taken</t>
   </si>
@@ -226,6 +225,9 @@
   </si>
   <si>
     <t>In beheersomgeving gebruikers die verkoper willen worden goed kunnen keuren</t>
+  </si>
+  <si>
+    <t>Gegevenspagina op profiel.php bij zetten</t>
   </si>
 </sst>
 </file>
@@ -304,7 +306,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -320,7 +322,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -618,21 +620,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341DCF5F-E2BF-41A3-B0D1-762933A4747F}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="41.109375" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -652,14 +654,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,7 +674,7 @@
       </c>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -683,7 +685,7 @@
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -694,7 +696,7 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -705,7 +707,7 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -716,7 +718,7 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -727,7 +729,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -738,7 +740,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -749,7 +751,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -760,7 +762,7 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -769,7 +771,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -780,7 +782,7 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -791,7 +793,7 @@
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -801,7 +803,7 @@
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -811,14 +813,14 @@
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
     </row>
-    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -828,14 +830,14 @@
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
@@ -845,7 +847,7 @@
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -855,7 +857,7 @@
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
@@ -865,7 +867,7 @@
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -875,11 +877,11 @@
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -889,7 +891,7 @@
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
@@ -899,14 +901,14 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>25</v>
       </c>
@@ -916,7 +918,7 @@
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>26</v>
       </c>
@@ -926,7 +928,7 @@
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -936,7 +938,7 @@
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
@@ -946,49 +948,47 @@
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
       </c>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
-      <c r="G34" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G35" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -996,46 +996,46 @@
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
     </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
     </row>
-    <row r="38" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>33</v>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
     </row>
-    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
+    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
     </row>
-    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
     </row>
-    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1043,36 +1043,36 @@
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
     </row>
-    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>37</v>
+    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
     </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43">
-        <v>0</v>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
     </row>
-    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
     </row>
-    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1080,56 +1080,56 @@
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>40</v>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
     </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>60</v>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="9">
-        <v>1</v>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
     </row>
-    <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
+        <v>43</v>
+      </c>
+      <c r="B49" s="9">
+        <v>1</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
     </row>
-    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
     </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1137,9 +1137,9 @@
       <c r="D51" s="13"/>
       <c r="E51" s="13"/>
     </row>
-    <row r="52" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1147,9 +1147,9 @@
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1157,38 +1157,48 @@
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
     </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
     </row>
-    <row r="56" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B64" s="12">
-        <f>SUM(B2:B56)</f>
-        <v>89</v>
+        <f>SUM(B2:B57)</f>
+        <v>92</v>
       </c>
       <c r="D64" s="10" t="s">
         <v>63</v>

</xml_diff>